<commit_message>
active links set in navbar
</commit_message>
<xml_diff>
--- a/src/Presentation/Adni.WebApi/Imports/sip.xlsx
+++ b/src/Presentation/Adni.WebApi/Imports/sip.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VisualStudio\Adni\src\Presentation\Adni.WebApi\Imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A088331-3DF5-4E84-9DD9-F2600C49BBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0EC7AB-10F4-47B2-9FD5-5D8CF2CE34B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="223">
   <si>
     <t>SEXE</t>
   </si>
@@ -114,12 +114,6 @@
     <t>kuatetanguy@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">M </t>
-  </si>
-  <si>
-    <t>TTI</t>
-  </si>
-  <si>
     <t>UNIVERSITE CATHOLIQUE</t>
   </si>
   <si>
@@ -451,9 +445,6 @@
   </si>
   <si>
     <t>syntychewang1@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F </t>
   </si>
   <si>
     <t>NGUENG NSOULI MELODIE NOELLE</t>
@@ -767,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -797,10 +788,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -809,23 +818,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1110,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,162 +1114,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
     </row>
     <row r="3" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="17" t="s">
+      <c r="O4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
     </row>
     <row r="5" spans="1:24" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="15" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15" t="s">
+      <c r="K5" s="18"/>
+      <c r="L5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="15"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14" t="s">
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15" t="s">
+      <c r="R5" s="18"/>
+      <c r="S5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="15"/>
-      <c r="U5" s="14" t="s">
+      <c r="T5" s="21"/>
+      <c r="U5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="V5" s="14"/>
-      <c r="W5" s="16" t="s">
+      <c r="V5" s="18"/>
+      <c r="W5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="16"/>
+      <c r="X5" s="22"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1383,7 +1377,7 @@
         <v>16</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J8" s="5">
         <v>2013</v>
@@ -1399,7 +1393,7 @@
       </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1413,21 +1407,21 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J9" s="5">
         <v>2020</v>
@@ -1443,7 +1437,7 @@
       </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
@@ -1457,21 +1451,21 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>35</v>
+      <c r="I10" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="J10" s="5">
         <v>2017</v>
@@ -1495,21 +1489,21 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>35</v>
+      <c r="I11" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="J11" s="5">
         <v>2017</v>
@@ -1525,11 +1519,11 @@
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R11" s="5"/>
       <c r="S11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="5" t="s">
@@ -1541,21 +1535,21 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J12" s="5">
         <v>2018</v>
@@ -1567,19 +1561,19 @@
       <c r="M12" s="5"/>
       <c r="N12" s="9"/>
       <c r="O12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T12" s="5"/>
       <c r="U12" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="7"/>
@@ -1587,21 +1581,21 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J13" s="5">
         <v>2015</v>
@@ -1617,11 +1611,11 @@
       </c>
       <c r="P13" s="5"/>
       <c r="Q13" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R13" s="5"/>
       <c r="S13" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T13" s="5"/>
       <c r="U13" s="5" t="s">
@@ -1629,27 +1623,27 @@
       </c>
       <c r="V13" s="5"/>
       <c r="W13" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X13" s="7"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>51</v>
+      <c r="I14" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="J14" s="5">
         <v>2017</v>
@@ -1665,11 +1659,11 @@
       </c>
       <c r="P14" s="5"/>
       <c r="Q14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T14" s="5"/>
       <c r="U14" s="5" t="s">
@@ -1681,21 +1675,21 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>51</v>
+      <c r="I15" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="J15" s="5">
         <v>2020</v>
@@ -1711,7 +1705,7 @@
       </c>
       <c r="P15" s="5"/>
       <c r="Q15" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
@@ -1725,18 +1719,18 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>22</v>
@@ -1746,45 +1740,45 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="9"/>
       <c r="O16" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="P16" s="5"/>
       <c r="Q16" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
       <c r="W16" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="X16" s="7"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J17" s="5">
@@ -1801,11 +1795,11 @@
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R17" s="5"/>
       <c r="S17" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="T17" s="5"/>
       <c r="U17" s="5" t="s">
@@ -1817,13 +1811,13 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1831,7 +1825,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J18" s="5">
         <v>2019</v>
@@ -1847,7 +1841,7 @@
       </c>
       <c r="P18" s="5"/>
       <c r="Q18" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
@@ -1861,18 +1855,18 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
-        <v>34</v>
+      <c r="H19" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>22</v>
@@ -1891,7 +1885,7 @@
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
@@ -1905,18 +1899,18 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>17</v>
@@ -1943,7 +1937,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1951,11 +1945,11 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J21" s="5">
         <v>2017</v>
@@ -1971,7 +1965,7 @@
       </c>
       <c r="P21" s="5"/>
       <c r="Q21" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
@@ -1983,13 +1977,13 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -2023,20 +2017,20 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>17</v>
       </c>
       <c r="J23" s="5">
@@ -2063,21 +2057,21 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="5" t="s">
-        <v>79</v>
+      <c r="I24" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="J24" s="5">
         <v>2021</v>
@@ -2093,7 +2087,7 @@
       </c>
       <c r="P24" s="5"/>
       <c r="Q24" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
@@ -2103,27 +2097,27 @@
       </c>
       <c r="V24" s="5"/>
       <c r="W24" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X24" s="7"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>79</v>
+      <c r="I25" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="J25" s="5">
         <v>2020</v>
@@ -2139,7 +2133,7 @@
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
@@ -2153,21 +2147,21 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J26" s="5">
         <v>2021</v>
@@ -2195,13 +2189,13 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2225,7 +2219,7 @@
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
@@ -2239,21 +2233,21 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J28" s="5">
         <v>2021</v>
@@ -2269,7 +2263,7 @@
       </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
@@ -2283,21 +2277,21 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J29" s="5">
         <v>2017</v>
@@ -2325,21 +2319,21 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J30" s="5">
         <v>2017</v>
@@ -2355,7 +2349,7 @@
       </c>
       <c r="P30" s="5"/>
       <c r="Q30" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
@@ -2369,21 +2363,21 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J31" s="5">
         <v>2019</v>
@@ -2399,7 +2393,7 @@
       </c>
       <c r="P31" s="5"/>
       <c r="Q31" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
@@ -2413,21 +2407,21 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J32" s="5">
         <v>2020</v>
@@ -2441,7 +2435,7 @@
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
@@ -2455,21 +2449,21 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J33" s="5">
         <v>2020</v>
@@ -2497,13 +2491,13 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -2511,7 +2505,7 @@
         <v>16</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J34" s="5">
         <v>2016</v>
@@ -2527,7 +2521,7 @@
       </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
@@ -2541,21 +2535,21 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J35" s="5">
         <v>2019</v>
@@ -2571,7 +2565,7 @@
       </c>
       <c r="P35" s="5"/>
       <c r="Q35" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
@@ -2585,13 +2579,13 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -2599,7 +2593,7 @@
         <v>16</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J36" s="5">
         <v>2019</v>
@@ -2627,18 +2621,18 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>22</v>
@@ -2657,7 +2651,7 @@
       </c>
       <c r="P37" s="5"/>
       <c r="Q37" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
@@ -2671,21 +2665,21 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J38" s="5">
         <v>2015</v>
@@ -2697,11 +2691,11 @@
       <c r="M38" s="5"/>
       <c r="N38" s="9"/>
       <c r="O38" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P38" s="5"/>
       <c r="Q38" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
@@ -2715,21 +2709,21 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J39" s="10">
         <v>2018</v>
@@ -2741,7 +2735,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="9"/>
       <c r="O39" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
@@ -2757,13 +2751,13 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -2778,7 +2772,7 @@
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="9"/>
@@ -2791,7 +2785,7 @@
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
       <c r="U40" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V40" s="5"/>
       <c r="W40" s="7"/>
@@ -2799,21 +2793,21 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="5" t="s">
-        <v>34</v>
+      <c r="H41" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J41" s="5">
         <v>2012</v>
@@ -2841,21 +2835,21 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="5" t="s">
-        <v>34</v>
+      <c r="H42" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J42" s="5">
         <v>2015</v>
@@ -2883,21 +2877,21 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="5" t="s">
-        <v>142</v>
+      <c r="H43" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J43" s="5">
         <v>2021</v>
@@ -2907,7 +2901,7 @@
       <c r="M43" s="5"/>
       <c r="N43" s="9"/>
       <c r="O43" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
@@ -2915,7 +2909,7 @@
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
       <c r="U43" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V43" s="5"/>
       <c r="W43" s="7"/>
@@ -2923,21 +2917,21 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J44" s="5">
         <v>2021</v>
@@ -2947,7 +2941,7 @@
       <c r="M44" s="5"/>
       <c r="N44" s="9"/>
       <c r="O44" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
@@ -2955,7 +2949,7 @@
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
       <c r="U44" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V44" s="5"/>
       <c r="W44" s="7"/>
@@ -2963,21 +2957,21 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J45" s="5">
         <v>2012</v>
@@ -3005,21 +2999,21 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="5" t="s">
+      <c r="H46" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J46" s="5">
         <v>2019</v>
@@ -3039,7 +3033,7 @@
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V46" s="5"/>
       <c r="W46" s="7"/>
@@ -3047,17 +3041,17 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
-      <c r="H47" s="5" t="s">
+      <c r="H47" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I47" s="5" t="s">
@@ -3081,7 +3075,7 @@
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
       <c r="U47" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V47" s="5"/>
       <c r="W47" s="7"/>
@@ -3089,17 +3083,17 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
-      <c r="H48" s="5" t="s">
+      <c r="H48" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I48" s="5" t="s">
@@ -3119,7 +3113,7 @@
       </c>
       <c r="P48" s="5"/>
       <c r="Q48" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="R48" s="5"/>
       <c r="S48" s="5"/>
@@ -3133,13 +3127,13 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
@@ -3163,7 +3157,7 @@
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
@@ -3177,21 +3171,21 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J50" s="5">
         <v>2017</v>
@@ -3219,21 +3213,21 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
-      <c r="H51" s="5" t="s">
+      <c r="H51" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J51" s="5">
         <v>2020</v>
@@ -3261,17 +3255,17 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I52" s="5" t="s">
@@ -3291,7 +3285,7 @@
       </c>
       <c r="P52" s="5"/>
       <c r="Q52" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="R52" s="5"/>
       <c r="S52" s="5"/>
@@ -3305,21 +3299,21 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
-      <c r="H53" s="5" t="s">
+      <c r="H53" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J53" s="5">
         <v>2019</v>
@@ -3347,7 +3341,7 @@
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -3359,7 +3353,7 @@
         <v>16</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J54" s="5">
         <v>2017</v>
@@ -3387,21 +3381,21 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
-      <c r="H55" s="5" t="s">
-        <v>34</v>
+      <c r="H55" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J55" s="5">
         <v>2017</v>
@@ -3421,7 +3415,7 @@
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
       <c r="U55" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V55" s="5"/>
       <c r="W55" s="7"/>
@@ -3429,33 +3423,33 @@
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
-      <c r="H56" s="5" t="s">
-        <v>34</v>
+      <c r="H56" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J56" s="5">
         <v>2020</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="M56" s="5"/>
       <c r="N56" s="9"/>
       <c r="O56" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P56" s="5"/>
       <c r="Q56" s="5"/>
@@ -3471,28 +3465,28 @@
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
-      <c r="H57" s="5" t="s">
-        <v>34</v>
+      <c r="H57" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J57" s="5">
         <v>2018</v>
       </c>
       <c r="K57" s="5"/>
       <c r="L57" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="M57" s="5"/>
       <c r="N57" s="9"/>
@@ -3501,7 +3495,7 @@
       </c>
       <c r="P57" s="5"/>
       <c r="Q57" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
@@ -3515,28 +3509,28 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
-      <c r="H58" s="5" t="s">
-        <v>34</v>
+      <c r="H58" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J58" s="5">
         <v>2018</v>
       </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M58" s="5"/>
       <c r="N58" s="9"/>
@@ -3545,7 +3539,7 @@
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="R58" s="5"/>
       <c r="S58" s="5"/>
@@ -3559,18 +3553,18 @@
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>22</v>
@@ -3589,7 +3583,7 @@
       </c>
       <c r="P59" s="5"/>
       <c r="Q59" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="R59" s="5"/>
       <c r="S59" s="5"/>
@@ -3603,7 +3597,7 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -3611,11 +3605,11 @@
       <c r="E60" s="6"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
-      <c r="H60" s="5" t="s">
+      <c r="H60" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J60" s="5">
         <v>2019</v>
@@ -3631,7 +3625,7 @@
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="R60" s="5"/>
       <c r="S60" s="5"/>
@@ -3645,20 +3639,20 @@
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J61" s="5">
@@ -3675,7 +3669,7 @@
       </c>
       <c r="P61" s="5"/>
       <c r="Q61" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R61" s="5"/>
       <c r="S61" s="5"/>
@@ -3689,17 +3683,17 @@
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I62" s="5" t="s">
@@ -3719,7 +3713,7 @@
       </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="R62" s="5"/>
       <c r="S62" s="5"/>
@@ -3733,7 +3727,7 @@
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -3741,11 +3735,11 @@
       <c r="E63" s="6"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
-      <c r="H63" s="5" t="s">
+      <c r="H63" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J63" s="5">
         <v>2020</v>
@@ -3761,7 +3755,7 @@
       </c>
       <c r="P63" s="5"/>
       <c r="Q63" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="R63" s="5"/>
       <c r="S63" s="5"/>
@@ -3775,17 +3769,17 @@
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I64" s="5" t="s">
@@ -3805,7 +3799,7 @@
       </c>
       <c r="P64" s="5"/>
       <c r="Q64" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="R64" s="5"/>
       <c r="S64" s="5"/>
@@ -3819,17 +3813,17 @@
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I65" s="5" t="s">
@@ -3845,7 +3839,7 @@
       <c r="M65" s="5"/>
       <c r="N65" s="9"/>
       <c r="O65" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="P65" s="5"/>
       <c r="Q65" s="5"/>
@@ -3859,18 +3853,18 @@
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>17</v>
@@ -3889,7 +3883,7 @@
       </c>
       <c r="P66" s="5"/>
       <c r="Q66" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="R66" s="5"/>
       <c r="S66" s="5"/>
@@ -3903,18 +3897,18 @@
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>17</v>
@@ -3933,13 +3927,13 @@
       </c>
       <c r="P67" s="5"/>
       <c r="Q67" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="R67" s="5"/>
       <c r="S67" s="8"/>
       <c r="T67" s="8"/>
       <c r="U67" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V67" s="5"/>
       <c r="W67" s="8"/>
@@ -3947,13 +3941,13 @@
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
@@ -3961,7 +3955,7 @@
         <v>16</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J68" s="5">
         <v>2015</v>
@@ -3977,13 +3971,13 @@
       </c>
       <c r="P68" s="5"/>
       <c r="Q68" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="R68" s="5"/>
       <c r="S68" s="8"/>
       <c r="T68" s="8"/>
       <c r="U68" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V68" s="5"/>
       <c r="W68" s="8"/>
@@ -3991,13 +3985,13 @@
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
@@ -4005,7 +3999,7 @@
         <v>16</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J69" s="5">
         <v>2012</v>
@@ -4021,7 +4015,7 @@
       </c>
       <c r="P69" s="5"/>
       <c r="Q69" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R69" s="5"/>
       <c r="S69" s="8"/>
@@ -4035,13 +4029,13 @@
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -4049,7 +4043,7 @@
         <v>16</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J70" s="5">
         <v>2018</v>
@@ -4065,13 +4059,13 @@
       </c>
       <c r="P70" s="5"/>
       <c r="Q70" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="R70" s="5"/>
       <c r="S70" s="8"/>
       <c r="T70" s="8"/>
       <c r="U70" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V70" s="5"/>
       <c r="W70" s="8"/>
@@ -4079,13 +4073,13 @@
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
@@ -4093,7 +4087,7 @@
         <v>16</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J71" s="5">
         <v>2014</v>
@@ -4109,7 +4103,7 @@
       </c>
       <c r="P71" s="5"/>
       <c r="Q71" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="R71" s="5"/>
       <c r="S71" s="8"/>
@@ -4123,13 +4117,13 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
@@ -4137,7 +4131,7 @@
         <v>16</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J72" s="5">
         <v>2013</v>
@@ -4153,7 +4147,7 @@
       </c>
       <c r="P72" s="5"/>
       <c r="Q72" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="R72" s="5"/>
       <c r="S72" s="8"/>
@@ -4165,13 +4159,13 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
@@ -4179,7 +4173,7 @@
         <v>16</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J73" s="5">
         <v>2015</v>
@@ -4191,7 +4185,7 @@
       <c r="M73" s="5"/>
       <c r="N73" s="9"/>
       <c r="O73" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="P73" s="5"/>
       <c r="Q73" s="5"/>
@@ -4207,13 +4201,13 @@
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
@@ -4233,7 +4227,7 @@
       <c r="M74" s="5"/>
       <c r="N74" s="9"/>
       <c r="O74" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="P74" s="5"/>
       <c r="Q74" s="5"/>
@@ -4249,13 +4243,13 @@
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
@@ -4263,7 +4257,7 @@
         <v>16</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J75" s="5">
         <v>2019</v>
@@ -4283,580 +4277,486 @@
       <c r="S75" s="8"/>
       <c r="T75" s="8"/>
       <c r="U75" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V75" s="5"/>
       <c r="W75" s="8"/>
       <c r="X75" s="8"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="22"/>
-      <c r="J76" s="19"/>
-      <c r="K76" s="19"/>
-      <c r="L76" s="22"/>
-      <c r="M76" s="22"/>
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
       <c r="N76" s="3"/>
-      <c r="O76" s="19"/>
-      <c r="P76" s="19"/>
-      <c r="Q76" s="19"/>
-      <c r="R76" s="19"/>
-      <c r="U76" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="V76" s="19"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="14"/>
+      <c r="Q76" s="14"/>
+      <c r="R76" s="14"/>
+      <c r="U76" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V76" s="14"/>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="22"/>
-      <c r="G77" s="22"/>
-      <c r="J77" s="19"/>
-      <c r="K77" s="19"/>
-      <c r="L77" s="22"/>
-      <c r="M77" s="22"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
       <c r="N77" s="3"/>
-      <c r="O77" s="19"/>
-      <c r="P77" s="19"/>
-      <c r="Q77" s="19"/>
-      <c r="R77" s="19"/>
-      <c r="U77" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="V77" s="19"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+      <c r="Q77" s="14"/>
+      <c r="R77" s="14"/>
+      <c r="U77" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V77" s="14"/>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A78" s="20"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="22"/>
-      <c r="J78" s="19"/>
-      <c r="K78" s="19"/>
-      <c r="L78" s="22"/>
-      <c r="M78" s="22"/>
+      <c r="A78" s="16"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
       <c r="N78" s="3"/>
-      <c r="O78" s="19"/>
-      <c r="P78" s="19"/>
-      <c r="Q78" s="19"/>
-      <c r="R78" s="19"/>
-      <c r="U78" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="V78" s="19"/>
+      <c r="O78" s="14"/>
+      <c r="P78" s="14"/>
+      <c r="Q78" s="14"/>
+      <c r="R78" s="14"/>
+      <c r="U78" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V78" s="14"/>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="22"/>
-      <c r="J79" s="19"/>
-      <c r="K79" s="19"/>
-      <c r="L79" s="22"/>
-      <c r="M79" s="22"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
       <c r="N79" s="3"/>
-      <c r="O79" s="19"/>
-      <c r="P79" s="19"/>
-      <c r="Q79" s="19"/>
-      <c r="R79" s="19"/>
-      <c r="U79" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="V79" s="19"/>
+      <c r="O79" s="14"/>
+      <c r="P79" s="14"/>
+      <c r="Q79" s="14"/>
+      <c r="R79" s="14"/>
+      <c r="U79" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V79" s="14"/>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="J80" s="19"/>
-      <c r="K80" s="19"/>
-      <c r="L80" s="22"/>
-      <c r="M80" s="22"/>
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
       <c r="N80" s="3"/>
-      <c r="O80" s="19"/>
-      <c r="P80" s="19"/>
-      <c r="Q80" s="19"/>
-      <c r="R80" s="19"/>
-      <c r="U80" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="V80" s="19"/>
+      <c r="O80" s="14"/>
+      <c r="P80" s="14"/>
+      <c r="Q80" s="14"/>
+      <c r="R80" s="14"/>
+      <c r="U80" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="22"/>
-      <c r="G81" s="22"/>
-      <c r="J81" s="19"/>
-      <c r="K81" s="19"/>
-      <c r="L81" s="22"/>
-      <c r="M81" s="22"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
       <c r="N81" s="3"/>
-      <c r="O81" s="19"/>
-      <c r="P81" s="19"/>
-      <c r="Q81" s="19"/>
-      <c r="R81" s="19"/>
-      <c r="U81" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="V81" s="19"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="14"/>
+      <c r="Q81" s="14"/>
+      <c r="R81" s="14"/>
+      <c r="U81" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V81" s="14"/>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="22"/>
-      <c r="G82" s="22"/>
-      <c r="J82" s="19"/>
-      <c r="K82" s="19"/>
-      <c r="L82" s="22"/>
-      <c r="M82" s="22"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
       <c r="N82" s="3"/>
-      <c r="O82" s="19"/>
-      <c r="P82" s="19"/>
-      <c r="Q82" s="19"/>
-      <c r="R82" s="19"/>
-      <c r="U82" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="V82" s="19"/>
+      <c r="O82" s="14"/>
+      <c r="P82" s="14"/>
+      <c r="Q82" s="14"/>
+      <c r="R82" s="14"/>
+      <c r="U82" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V82" s="14"/>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J83" s="19"/>
-      <c r="K83" s="19"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J84" s="19"/>
-      <c r="K84" s="19"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J85" s="19"/>
-      <c r="K85" s="19"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J86" s="19"/>
-      <c r="K86" s="19"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J87" s="19"/>
-      <c r="K87" s="19"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J88" s="19"/>
-      <c r="K88" s="19"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J89" s="19"/>
-      <c r="K89" s="19"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J90" s="19"/>
-      <c r="K90" s="19"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J91" s="19"/>
-      <c r="K91" s="19"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J92" s="19"/>
-      <c r="K92" s="19"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J93" s="19"/>
-      <c r="K93" s="19"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J94" s="19"/>
-      <c r="K94" s="19"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="14"/>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J95" s="19"/>
-      <c r="K95" s="19"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J96" s="19"/>
-      <c r="K96" s="19"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="14"/>
     </row>
     <row r="97" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J97" s="19"/>
-      <c r="K97" s="19"/>
+      <c r="J97" s="14"/>
+      <c r="K97" s="14"/>
     </row>
     <row r="98" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J98" s="19"/>
-      <c r="K98" s="19"/>
+      <c r="J98" s="14"/>
+      <c r="K98" s="14"/>
     </row>
     <row r="99" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J99" s="19"/>
-      <c r="K99" s="19"/>
+      <c r="J99" s="14"/>
+      <c r="K99" s="14"/>
     </row>
     <row r="100" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J100" s="19"/>
-      <c r="K100" s="19"/>
+      <c r="J100" s="14"/>
+      <c r="K100" s="14"/>
     </row>
     <row r="101" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J101" s="19"/>
-      <c r="K101" s="19"/>
+      <c r="J101" s="14"/>
+      <c r="K101" s="14"/>
     </row>
     <row r="102" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J102" s="19"/>
-      <c r="K102" s="19"/>
+      <c r="J102" s="14"/>
+      <c r="K102" s="14"/>
     </row>
     <row r="103" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J103" s="19"/>
-      <c r="K103" s="19"/>
+      <c r="J103" s="14"/>
+      <c r="K103" s="14"/>
     </row>
     <row r="104" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J104" s="19"/>
-      <c r="K104" s="19"/>
+      <c r="J104" s="14"/>
+      <c r="K104" s="14"/>
     </row>
     <row r="105" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J105" s="19"/>
-      <c r="K105" s="19"/>
+      <c r="J105" s="14"/>
+      <c r="K105" s="14"/>
     </row>
     <row r="106" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J106" s="19"/>
-      <c r="K106" s="19"/>
+      <c r="J106" s="14"/>
+      <c r="K106" s="14"/>
     </row>
     <row r="107" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J107" s="19"/>
-      <c r="K107" s="19"/>
+      <c r="J107" s="14"/>
+      <c r="K107" s="14"/>
     </row>
     <row r="108" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J108" s="19"/>
-      <c r="K108" s="19"/>
+      <c r="J108" s="14"/>
+      <c r="K108" s="14"/>
     </row>
     <row r="109" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J109" s="19"/>
-      <c r="K109" s="19"/>
+      <c r="J109" s="14"/>
+      <c r="K109" s="14"/>
     </row>
     <row r="110" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J110" s="19"/>
-      <c r="K110" s="19"/>
+      <c r="J110" s="14"/>
+      <c r="K110" s="14"/>
     </row>
     <row r="111" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J111" s="19"/>
-      <c r="K111" s="19"/>
+      <c r="J111" s="14"/>
+      <c r="K111" s="14"/>
     </row>
     <row r="112" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J112" s="19"/>
-      <c r="K112" s="19"/>
+      <c r="J112" s="14"/>
+      <c r="K112" s="14"/>
     </row>
     <row r="113" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J113" s="19"/>
-      <c r="K113" s="19"/>
+      <c r="J113" s="14"/>
+      <c r="K113" s="14"/>
     </row>
     <row r="114" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J114" s="19"/>
-      <c r="K114" s="19"/>
+      <c r="J114" s="14"/>
+      <c r="K114" s="14"/>
     </row>
     <row r="115" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J115" s="19"/>
-      <c r="K115" s="19"/>
+      <c r="J115" s="14"/>
+      <c r="K115" s="14"/>
     </row>
     <row r="116" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J116" s="19"/>
-      <c r="K116" s="19"/>
+      <c r="J116" s="14"/>
+      <c r="K116" s="14"/>
     </row>
     <row r="117" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J117" s="19"/>
-      <c r="K117" s="19"/>
+      <c r="J117" s="14"/>
+      <c r="K117" s="14"/>
     </row>
     <row r="118" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J118" s="19"/>
-      <c r="K118" s="19"/>
+      <c r="J118" s="14"/>
+      <c r="K118" s="14"/>
     </row>
     <row r="119" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J119" s="19"/>
-      <c r="K119" s="19"/>
+      <c r="J119" s="14"/>
+      <c r="K119" s="14"/>
     </row>
     <row r="120" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J120" s="19"/>
-      <c r="K120" s="19"/>
+      <c r="J120" s="14"/>
+      <c r="K120" s="14"/>
     </row>
     <row r="121" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J121" s="19"/>
-      <c r="K121" s="19"/>
+      <c r="J121" s="14"/>
+      <c r="K121" s="14"/>
     </row>
     <row r="122" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J122" s="19"/>
-      <c r="K122" s="19"/>
+      <c r="J122" s="14"/>
+      <c r="K122" s="14"/>
     </row>
     <row r="123" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J123" s="19"/>
-      <c r="K123" s="19"/>
+      <c r="J123" s="14"/>
+      <c r="K123" s="14"/>
     </row>
     <row r="124" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J124" s="19"/>
-      <c r="K124" s="19"/>
+      <c r="J124" s="14"/>
+      <c r="K124" s="14"/>
     </row>
     <row r="125" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J125" s="19"/>
-      <c r="K125" s="19"/>
+      <c r="J125" s="14"/>
+      <c r="K125" s="14"/>
     </row>
     <row r="126" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J126" s="19"/>
-      <c r="K126" s="19"/>
+      <c r="J126" s="14"/>
+      <c r="K126" s="14"/>
     </row>
     <row r="127" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J127" s="19"/>
-      <c r="K127" s="19"/>
+      <c r="J127" s="14"/>
+      <c r="K127" s="14"/>
     </row>
     <row r="128" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J128" s="19"/>
-      <c r="K128" s="19"/>
+      <c r="J128" s="14"/>
+      <c r="K128" s="14"/>
     </row>
     <row r="129" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J129" s="19"/>
-      <c r="K129" s="19"/>
+      <c r="J129" s="14"/>
+      <c r="K129" s="14"/>
     </row>
     <row r="130" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J130" s="19"/>
-      <c r="K130" s="19"/>
+      <c r="J130" s="14"/>
+      <c r="K130" s="14"/>
     </row>
     <row r="131" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J131" s="19"/>
-      <c r="K131" s="19"/>
+      <c r="J131" s="14"/>
+      <c r="K131" s="14"/>
     </row>
     <row r="132" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J132" s="19"/>
-      <c r="K132" s="19"/>
+      <c r="J132" s="14"/>
+      <c r="K132" s="14"/>
     </row>
     <row r="133" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J133" s="19"/>
-      <c r="K133" s="19"/>
+      <c r="J133" s="14"/>
+      <c r="K133" s="14"/>
     </row>
     <row r="134" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J134" s="19"/>
-      <c r="K134" s="19"/>
+      <c r="J134" s="14"/>
+      <c r="K134" s="14"/>
     </row>
     <row r="135" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J135" s="19"/>
-      <c r="K135" s="19"/>
+      <c r="J135" s="14"/>
+      <c r="K135" s="14"/>
     </row>
     <row r="136" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J136" s="19"/>
-      <c r="K136" s="19"/>
+      <c r="J136" s="14"/>
+      <c r="K136" s="14"/>
     </row>
     <row r="137" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J137" s="19"/>
-      <c r="K137" s="19"/>
+      <c r="J137" s="14"/>
+      <c r="K137" s="14"/>
     </row>
     <row r="138" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J138" s="19"/>
-      <c r="K138" s="19"/>
+      <c r="J138" s="14"/>
+      <c r="K138" s="14"/>
     </row>
     <row r="139" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J139" s="19"/>
-      <c r="K139" s="19"/>
+      <c r="J139" s="14"/>
+      <c r="K139" s="14"/>
     </row>
     <row r="140" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J140" s="19"/>
-      <c r="K140" s="19"/>
+      <c r="J140" s="14"/>
+      <c r="K140" s="14"/>
     </row>
     <row r="141" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J141" s="19"/>
-      <c r="K141" s="19"/>
+      <c r="J141" s="14"/>
+      <c r="K141" s="14"/>
     </row>
     <row r="142" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J142" s="19"/>
-      <c r="K142" s="19"/>
+      <c r="J142" s="14"/>
+      <c r="K142" s="14"/>
     </row>
     <row r="143" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J143" s="19"/>
-      <c r="K143" s="19"/>
+      <c r="J143" s="14"/>
+      <c r="K143" s="14"/>
     </row>
     <row r="144" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J144" s="19"/>
-      <c r="K144" s="19"/>
+      <c r="J144" s="14"/>
+      <c r="K144" s="14"/>
     </row>
     <row r="145" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J145" s="19"/>
-      <c r="K145" s="19"/>
+      <c r="J145" s="14"/>
+      <c r="K145" s="14"/>
     </row>
     <row r="146" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J146" s="19"/>
-      <c r="K146" s="19"/>
+      <c r="J146" s="14"/>
+      <c r="K146" s="14"/>
     </row>
     <row r="147" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J147" s="19"/>
-      <c r="K147" s="19"/>
+      <c r="J147" s="14"/>
+      <c r="K147" s="14"/>
     </row>
     <row r="148" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J148" s="19"/>
-      <c r="K148" s="19"/>
+      <c r="J148" s="14"/>
+      <c r="K148" s="14"/>
     </row>
     <row r="149" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J149" s="19"/>
-      <c r="K149" s="19"/>
+      <c r="J149" s="14"/>
+      <c r="K149" s="14"/>
     </row>
     <row r="150" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J150" s="19"/>
-      <c r="K150" s="19"/>
+      <c r="J150" s="14"/>
+      <c r="K150" s="14"/>
     </row>
     <row r="151" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J151" s="19"/>
-      <c r="K151" s="19"/>
+      <c r="J151" s="14"/>
+      <c r="K151" s="14"/>
     </row>
     <row r="152" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J152" s="19"/>
-      <c r="K152" s="19"/>
+      <c r="J152" s="14"/>
+      <c r="K152" s="14"/>
     </row>
     <row r="153" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J153" s="19"/>
-      <c r="K153" s="19"/>
+      <c r="J153" s="14"/>
+      <c r="K153" s="14"/>
     </row>
     <row r="154" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J154" s="19"/>
-      <c r="K154" s="19"/>
+      <c r="J154" s="14"/>
+      <c r="K154" s="14"/>
     </row>
     <row r="155" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J155" s="19"/>
-      <c r="K155" s="19"/>
+      <c r="J155" s="14"/>
+      <c r="K155" s="14"/>
     </row>
     <row r="156" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J156" s="19"/>
-      <c r="K156" s="19"/>
+      <c r="J156" s="14"/>
+      <c r="K156" s="14"/>
     </row>
     <row r="157" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J157" s="19"/>
-      <c r="K157" s="19"/>
+      <c r="J157" s="14"/>
+      <c r="K157" s="14"/>
     </row>
     <row r="158" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J158" s="19"/>
-      <c r="K158" s="19"/>
+      <c r="J158" s="14"/>
+      <c r="K158" s="14"/>
     </row>
     <row r="159" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J159" s="19"/>
-      <c r="K159" s="19"/>
+      <c r="J159" s="14"/>
+      <c r="K159" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="Q76:R76"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="Q78:R78"/>
-    <mergeCell ref="U79:V79"/>
-    <mergeCell ref="U80:V80"/>
-    <mergeCell ref="U81:V81"/>
-    <mergeCell ref="U82:V82"/>
-    <mergeCell ref="U76:V76"/>
-    <mergeCell ref="U77:V77"/>
-    <mergeCell ref="Q79:R79"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="O78:P78"/>
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="L80:M80"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="U78:V78"/>
-    <mergeCell ref="Q80:R80"/>
-    <mergeCell ref="Q81:R81"/>
-    <mergeCell ref="Q82:R82"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="J155:K155"/>
-    <mergeCell ref="J156:K156"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="J158:K158"/>
-    <mergeCell ref="J159:K159"/>
-    <mergeCell ref="J149:K149"/>
-    <mergeCell ref="J150:K150"/>
-    <mergeCell ref="J151:K151"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="J154:K154"/>
-    <mergeCell ref="J143:K143"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="J145:K145"/>
-    <mergeCell ref="J146:K146"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="J148:K148"/>
-    <mergeCell ref="J137:K137"/>
-    <mergeCell ref="J138:K138"/>
-    <mergeCell ref="J139:K139"/>
-    <mergeCell ref="J140:K140"/>
-    <mergeCell ref="J141:K141"/>
-    <mergeCell ref="J142:K142"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="J133:K133"/>
-    <mergeCell ref="J134:K134"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J125:K125"/>
-    <mergeCell ref="J126:K126"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J128:K128"/>
-    <mergeCell ref="J129:K129"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J119:K119"/>
-    <mergeCell ref="J120:K120"/>
-    <mergeCell ref="J121:K121"/>
-    <mergeCell ref="J122:K122"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="J124:K124"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J115:K115"/>
-    <mergeCell ref="J116:K116"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J107:K107"/>
-    <mergeCell ref="J108:K108"/>
-    <mergeCell ref="J109:K109"/>
-    <mergeCell ref="J110:K110"/>
-    <mergeCell ref="J111:K111"/>
-    <mergeCell ref="J112:K112"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="J95:K95"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="J97:K97"/>
-    <mergeCell ref="J98:K98"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="J91:K91"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="A1:X3"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O5:P5"/>
     <mergeCell ref="J83:K83"/>
     <mergeCell ref="J84:K84"/>
     <mergeCell ref="J85:K85"/>
@@ -4881,16 +4781,110 @@
     <mergeCell ref="O81:P81"/>
     <mergeCell ref="O82:P82"/>
     <mergeCell ref="O76:P76"/>
-    <mergeCell ref="A1:X3"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="J95:K95"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="J97:K97"/>
+    <mergeCell ref="J98:K98"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="J91:K91"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="J107:K107"/>
+    <mergeCell ref="J108:K108"/>
+    <mergeCell ref="J109:K109"/>
+    <mergeCell ref="J110:K110"/>
+    <mergeCell ref="J111:K111"/>
+    <mergeCell ref="J112:K112"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="J120:K120"/>
+    <mergeCell ref="J121:K121"/>
+    <mergeCell ref="J122:K122"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="J124:K124"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="J115:K115"/>
+    <mergeCell ref="J116:K116"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="J133:K133"/>
+    <mergeCell ref="J134:K134"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J125:K125"/>
+    <mergeCell ref="J126:K126"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J128:K128"/>
+    <mergeCell ref="J129:K129"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J143:K143"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="J145:K145"/>
+    <mergeCell ref="J146:K146"/>
+    <mergeCell ref="J147:K147"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="J137:K137"/>
+    <mergeCell ref="J138:K138"/>
+    <mergeCell ref="J139:K139"/>
+    <mergeCell ref="J140:K140"/>
+    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="J142:K142"/>
+    <mergeCell ref="J155:K155"/>
+    <mergeCell ref="J156:K156"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="J158:K158"/>
+    <mergeCell ref="J159:K159"/>
+    <mergeCell ref="J149:K149"/>
+    <mergeCell ref="J150:K150"/>
+    <mergeCell ref="J151:K151"/>
+    <mergeCell ref="J152:K152"/>
+    <mergeCell ref="J153:K153"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="O78:P78"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="U78:V78"/>
+    <mergeCell ref="Q80:R80"/>
+    <mergeCell ref="Q81:R81"/>
+    <mergeCell ref="Q82:R82"/>
+    <mergeCell ref="Q76:R76"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="Q78:R78"/>
+    <mergeCell ref="U79:V79"/>
+    <mergeCell ref="U80:V80"/>
+    <mergeCell ref="U81:V81"/>
+    <mergeCell ref="U82:V82"/>
+    <mergeCell ref="U76:V76"/>
+    <mergeCell ref="U77:V77"/>
+    <mergeCell ref="Q79:R79"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>